<commit_message>
All the Data, ready for Evaluation
</commit_message>
<xml_diff>
--- a/Auswertung_5.xlsx
+++ b/Auswertung_5.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>t(s)</t>
   </si>
@@ -396,1100 +396,1916 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B136"/>
+  <dimension ref="A1:D136"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>-1.56917258989519E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.80328373729942004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>3.3333333333333E-2</v>
       </c>
       <c r="B3" s="1">
         <v>1.25462414263486E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" s="1">
+        <v>3.3333333333333E-2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.80349723169067999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>6.6666666666666E-2</v>
       </c>
       <c r="B4" s="1">
         <v>2.6748537363709E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" s="1">
+        <v>6.6666666666666E-2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.80373193920673502</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>9.9999999999999006E-2</v>
       </c>
       <c r="B5" s="1">
         <v>4.0658783147942502E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" s="1">
+        <v>9.9999999999999006E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.803757334244252</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>0.133333333333332</v>
       </c>
       <c r="B6" s="1">
         <v>5.4814790357260001E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" s="1">
+        <v>0.133333333333332</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.80384151797098802</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>0.16666666666666599</v>
       </c>
       <c r="B7" s="1">
         <v>6.8675279321905605E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" s="1">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.80430496677215002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>0.2</v>
       </c>
       <c r="B8" s="1">
         <v>8.1602234331266496E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.80439173204367997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>0.233333333333333</v>
       </c>
       <c r="B9" s="1">
         <v>9.5479037813716403E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" s="1">
+        <v>0.233333333333333</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.80441452764601895</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>0.266666666666666</v>
       </c>
       <c r="B10" s="1">
         <v>0.108953146447252</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" s="1">
+        <v>0.266666666666666</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.80470917457312396</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>0.29999999999999899</v>
       </c>
       <c r="B11" s="1">
         <v>0.12276095132828101</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11" s="1">
+        <v>0.29999999999999899</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.804894950808691</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>0.33333333333333298</v>
       </c>
       <c r="B12" s="1">
         <v>0.135705630677325</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12" s="1">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.804882026478417</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>0.36666666666666597</v>
       </c>
       <c r="B13" s="1">
         <v>0.14879435540246</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13" s="1">
+        <v>0.36666666666666597</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.80491191148954</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="1">
         <v>0.39999999999999902</v>
       </c>
       <c r="B14" s="1">
         <v>0.16178205836965301</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14" s="1">
+        <v>0.39999999999999902</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.80491835445788695</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>0.43333333333333302</v>
       </c>
       <c r="B15" s="1">
         <v>0.174792991271397</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15" s="1">
+        <v>0.43333333333333302</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.80496680547065702</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="1">
         <v>0.46666666666666601</v>
       </c>
       <c r="B16" s="1">
         <v>0.187473138055442</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" s="1">
+        <v>0.46666666666666601</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.80491665551185898</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>0.5</v>
       </c>
       <c r="B17" s="1">
         <v>0.20052845894197999</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.80497743426704405</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>0.53333333333333299</v>
       </c>
       <c r="B18" s="1">
         <v>0.21302745687216401</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18" s="1">
+        <v>0.53333333333333299</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.80497859012111905</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>0.56666666666666599</v>
       </c>
       <c r="B19" s="1">
         <v>0.22585909664669801</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" s="1">
+        <v>0.56666666666666599</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.80491870164225399</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>0.59999999999999898</v>
       </c>
       <c r="B20" s="1">
         <v>0.23789922073581499</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20" s="1">
+        <v>0.59999999999999898</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.804907272702576</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>0.63333333333333197</v>
       </c>
       <c r="B21" s="1">
         <v>0.25058777467500198</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21" s="1">
+        <v>0.63333333333333197</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.80490613676012801</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>0.66666666666666696</v>
       </c>
       <c r="B22" s="1">
         <v>0.26317335052806701</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22" s="1">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.80458082646511397</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>0.7</v>
       </c>
       <c r="B23" s="1">
         <v>0.27534337290863697</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.80447717926470297</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="1">
         <v>0.73333333333333295</v>
       </c>
       <c r="B24" s="1">
         <v>0.28782441754802401</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24" s="1">
+        <v>0.73333333333333295</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.80437464226497402</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="1">
         <v>0.76666666666666605</v>
       </c>
       <c r="B25" s="1">
         <v>0.30008448758559197</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25" s="1">
+        <v>0.76666666666666605</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.80431386767394797</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="1">
         <v>0.79999999999999905</v>
       </c>
       <c r="B26" s="1">
         <v>0.30925974204585999</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26" s="1">
+        <v>0.79999999999999905</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.800969799746029</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="1">
         <v>0.83333333333333304</v>
       </c>
       <c r="B27" s="1">
         <v>0.32385463494220301</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27" s="1">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0.80395820772349502</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="1">
         <v>0.86666666666666603</v>
       </c>
       <c r="B28" s="1">
         <v>0.33569592363942202</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28" s="1">
+        <v>0.86666666666666603</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0.80081644278694297</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="1">
         <v>0.9</v>
       </c>
       <c r="B29" s="1">
         <v>0.34759181859258598</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0.80040437943874398</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="1">
         <v>0.93333333333333302</v>
       </c>
       <c r="B30" s="1">
         <v>0.35927007397446298</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30" s="1">
+        <v>0.93333333333333302</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0.80010350368905503</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="1">
         <v>0.96666666666666601</v>
       </c>
       <c r="B31" s="1">
         <v>0.37046556859221302</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31" s="1">
+        <v>0.96666666666666601</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.799828545191962</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="1">
         <v>1</v>
       </c>
       <c r="B32" s="1">
         <v>0.38165474946620598</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0.79937994493382802</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" s="1">
         <v>1.0333333333333301</v>
       </c>
       <c r="B33" s="1">
         <v>0.39360200203547402</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33" s="1">
+        <v>1.0333333333333301</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0.79901943253357799</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="1">
         <v>1.06666666666666</v>
       </c>
       <c r="B34" s="1">
         <v>0.40463820641739201</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34" s="1">
+        <v>1.06666666666666</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0.79862535865348305</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" s="1">
         <v>1.0999999999999901</v>
       </c>
       <c r="B35" s="1">
         <v>0.41578928615227601</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35" s="1">
+        <v>1.0999999999999901</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0.79849334285974305</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="1">
         <v>1.13333333333333</v>
       </c>
       <c r="B36" s="1">
         <v>0.426561342048009</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36" s="1">
+        <v>1.13333333333333</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0.79765611015978299</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" s="1">
         <v>1.1666666666666601</v>
       </c>
       <c r="B37" s="1">
         <v>0.43804218832317598</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37" s="1">
+        <v>1.1666666666666601</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0.797504927125959</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="1">
         <v>1.2</v>
       </c>
       <c r="B38" s="1">
         <v>0.449226755257149</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="C38" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0.79723591087500001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" s="1">
         <v>1.2333333333333301</v>
       </c>
       <c r="B39" s="1">
         <v>0.46007363201261198</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="C39" s="1">
+        <v>1.2333333333333301</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0.79688347454002395</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" s="1">
         <v>1.2666666666666599</v>
       </c>
       <c r="B40" s="1">
         <v>0.47079623022227401</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="C40" s="1">
+        <v>1.2666666666666599</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0.79643012027827897</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" s="1">
         <v>1.2999999999999901</v>
       </c>
       <c r="B41" s="1">
         <v>0.48113689769961498</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="C41" s="1">
+        <v>1.2999999999999901</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0.79598128169593896</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="1">
         <v>1.3333333333333299</v>
       </c>
       <c r="B42" s="1">
         <v>0.491604334206167</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="C42" s="1">
+        <v>1.3333333333333299</v>
+      </c>
+      <c r="D42" s="1">
+        <v>0.79542775566257795</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" s="1">
         <v>1.36666666666666</v>
       </c>
       <c r="B43" s="1">
         <v>0.50238239770219995</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="C43" s="1">
+        <v>1.36666666666666</v>
+      </c>
+      <c r="D43" s="1">
+        <v>0.79500789359917401</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="1">
         <v>1.4</v>
       </c>
       <c r="B44" s="1">
         <v>0.51236684738995597</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="C44" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0.79453721762075302</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="1">
         <v>1.43333333333333</v>
       </c>
       <c r="B45" s="1">
         <v>0.52258648571266397</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
+      <c r="C45" s="1">
+        <v>1.43333333333333</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0.79427451605581201</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="1">
         <v>1.4666666666666599</v>
       </c>
       <c r="B46" s="1">
         <v>0.53261589533607001</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="C46" s="1">
+        <v>1.4666666666666599</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0.79374564330887898</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" s="1">
         <v>1.5</v>
       </c>
       <c r="B47" s="1">
         <v>0.54238571753352205</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="C47" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0.79325794919630699</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="1">
         <v>1.5333333333333301</v>
       </c>
       <c r="B48" s="1">
         <v>0.55232686855270496</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="C48" s="1">
+        <v>1.5333333333333301</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0.79311513508231402</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="1">
         <v>1.56666666666666</v>
       </c>
       <c r="B49" s="1">
         <v>0.56218666814970897</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="C49" s="1">
+        <v>1.56666666666666</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0.79303636042452497</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" s="1">
         <v>1.5999999999999901</v>
       </c>
       <c r="B50" s="1">
         <v>0.57211284154091002</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="C50" s="1">
+        <v>1.5999999999999901</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0.79253653785176204</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" s="1">
         <v>1.63333333333333</v>
       </c>
       <c r="B51" s="1">
         <v>0.58144104463712798</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="C51" s="1">
+        <v>1.63333333333333</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0.79209826811471096</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" s="1">
         <v>1.6666666666666601</v>
       </c>
       <c r="B52" s="1">
         <v>0.590678149859996</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="C52" s="1">
+        <v>1.6666666666666601</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0.79152293472367596</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="1">
         <v>1.7</v>
       </c>
       <c r="B53" s="1">
         <v>0.60035032524245302</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="C53" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0.79114616487796896</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" s="1">
         <v>1.7333333333333301</v>
       </c>
       <c r="B54" s="1">
         <v>0.60928848058981699</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="C54" s="1">
+        <v>1.7333333333333301</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0.79092157207777003</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" s="1">
         <v>1.7666666666666599</v>
       </c>
       <c r="B55" s="1">
         <v>0.61856609274952801</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="C55" s="1">
+        <v>1.7666666666666599</v>
+      </c>
+      <c r="D55" s="1">
+        <v>0.79052262647425597</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" s="1">
         <v>1.7999999999999901</v>
       </c>
       <c r="B56" s="1">
         <v>0.62733850296184901</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
+      <c r="C56" s="1">
+        <v>1.7999999999999901</v>
+      </c>
+      <c r="D56" s="1">
+        <v>0.789952645789462</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" s="1">
         <v>1.8333333333333299</v>
       </c>
       <c r="B57" s="1">
         <v>0.63641094906863904</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="C57" s="1">
+        <v>1.8333333333333299</v>
+      </c>
+      <c r="D57" s="1">
+        <v>0.78981975172019503</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" s="1">
         <v>1.86666666666666</v>
       </c>
       <c r="B58" s="1">
         <v>0.645186415301505</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
+      <c r="C58" s="1">
+        <v>1.86666666666666</v>
+      </c>
+      <c r="D58" s="1">
+        <v>0.78974224537675297</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" s="1">
         <v>1.8999999999999899</v>
       </c>
       <c r="B59" s="1">
         <v>0.65366085792203699</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
+      <c r="C59" s="1">
+        <v>1.8999999999999899</v>
+      </c>
+      <c r="D59" s="1">
+        <v>0.78964250449069695</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" s="1">
         <v>1.93333333333333</v>
       </c>
       <c r="B60" s="1">
         <v>0.66193275212393998</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
+      <c r="C60" s="1">
+        <v>1.93333333333333</v>
+      </c>
+      <c r="D60" s="1">
+        <v>0.78971978028154</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" s="1">
         <v>1.9666666666666599</v>
       </c>
       <c r="B61" s="1">
         <v>0.67007023698743495</v>
       </c>
-    </row>
-    <row r="62" spans="1:2">
+      <c r="C61" s="1">
+        <v>1.9666666666666599</v>
+      </c>
+      <c r="D61" s="1">
+        <v>0.78983202011815201</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" s="1">
         <v>1.99999999999999</v>
       </c>
       <c r="B62" s="1">
         <v>0.67789893025022396</v>
       </c>
-    </row>
-    <row r="63" spans="1:2">
+      <c r="C62" s="1">
+        <v>1.99999999999999</v>
+      </c>
+      <c r="D62" s="1">
+        <v>0.79007475428317397</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" s="1">
         <v>2.0333333333333301</v>
       </c>
       <c r="B63" s="1">
         <v>0.68554018769294001</v>
       </c>
-    </row>
-    <row r="64" spans="1:2">
+      <c r="C63" s="1">
+        <v>2.0333333333333301</v>
+      </c>
+      <c r="D63" s="1">
+        <v>0.790530849826243</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" s="1">
         <v>2.0666666666666602</v>
       </c>
       <c r="B64" s="1">
         <v>0.69234334109484696</v>
       </c>
-    </row>
-    <row r="65" spans="1:2">
+      <c r="C64" s="1">
+        <v>2.0666666666666602</v>
+      </c>
+      <c r="D64" s="1">
+        <v>0.79158637296452705</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" s="1">
         <v>2.1</v>
       </c>
       <c r="B65" s="1">
         <v>0.69606193033911801</v>
       </c>
-    </row>
-    <row r="66" spans="1:2">
+      <c r="C65" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="D65" s="1">
+        <v>0.79580422649153104</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" s="1">
         <v>2.1333333333333302</v>
       </c>
       <c r="B66" s="1">
         <v>0.69917617529821596</v>
       </c>
-    </row>
-    <row r="67" spans="1:2">
+      <c r="C66" s="1">
+        <v>2.1333333333333302</v>
+      </c>
+      <c r="D66" s="1">
+        <v>0.800630084362705</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" s="1">
         <v>2.1666666666666599</v>
       </c>
       <c r="B67" s="1">
         <v>0.70161445426108704</v>
       </c>
-    </row>
-    <row r="68" spans="1:2">
+      <c r="C67" s="1">
+        <v>2.1666666666666599</v>
+      </c>
+      <c r="D67" s="1">
+        <v>0.80585607166590201</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" s="1">
         <v>2.19999999999999</v>
       </c>
       <c r="B68" s="1">
         <v>0.70376705497904501</v>
       </c>
-    </row>
-    <row r="69" spans="1:2">
+      <c r="C68" s="1">
+        <v>2.19999999999999</v>
+      </c>
+      <c r="D68" s="1">
+        <v>0.81118401719501598</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" s="1">
         <v>2.2333333333333298</v>
       </c>
       <c r="B69" s="1">
         <v>0.70559789731129197</v>
       </c>
-    </row>
-    <row r="70" spans="1:2">
+      <c r="C69" s="1">
+        <v>2.2333333333333298</v>
+      </c>
+      <c r="D69" s="1">
+        <v>0.81689062715024097</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" s="1">
         <v>2.2666666666666599</v>
       </c>
       <c r="B70" s="1">
         <v>0.70741776543618895</v>
       </c>
-    </row>
-    <row r="71" spans="1:2">
+      <c r="C70" s="1">
+        <v>2.2666666666666599</v>
+      </c>
+      <c r="D70" s="1">
+        <v>0.82284626858765997</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" s="1">
         <v>2.2999999999999901</v>
       </c>
       <c r="B71" s="1">
         <v>0.70865876178600296</v>
       </c>
-    </row>
-    <row r="72" spans="1:2">
+      <c r="C71" s="1">
+        <v>2.2999999999999901</v>
+      </c>
+      <c r="D71" s="1">
+        <v>0.82890472914241797</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" s="1">
         <v>2.3333333333333299</v>
       </c>
       <c r="B72" s="1">
         <v>0.70968686826550298</v>
       </c>
-    </row>
-    <row r="73" spans="1:2">
+      <c r="C72" s="1">
+        <v>2.3333333333333299</v>
+      </c>
+      <c r="D72" s="1">
+        <v>0.83511660386011299</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" s="1">
         <v>2.36666666666666</v>
       </c>
       <c r="B73" s="1">
         <v>0.71077971333752399</v>
       </c>
-    </row>
-    <row r="74" spans="1:2">
+      <c r="C73" s="1">
+        <v>2.36666666666666</v>
+      </c>
+      <c r="D73" s="1">
+        <v>0.84163537084856399</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" s="1">
         <v>2.3999999999999901</v>
       </c>
       <c r="B74" s="1">
         <v>0.71167969677992604</v>
       </c>
-    </row>
-    <row r="75" spans="1:2">
+      <c r="C74" s="1">
+        <v>2.3999999999999901</v>
+      </c>
+      <c r="D74" s="1">
+        <v>0.84804784158873803</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" s="1">
         <v>2.43333333333333</v>
       </c>
       <c r="B75" s="1">
         <v>0.71245114814411103</v>
       </c>
-    </row>
-    <row r="76" spans="1:2">
+      <c r="C75" s="1">
+        <v>2.43333333333333</v>
+      </c>
+      <c r="D75" s="1">
+        <v>0.85473691141735197</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" s="1">
         <v>2.4666666666666601</v>
       </c>
       <c r="B76" s="1">
         <v>0.713051379136733</v>
       </c>
-    </row>
-    <row r="77" spans="1:2">
+      <c r="C76" s="1">
+        <v>2.4666666666666601</v>
+      </c>
+      <c r="D76" s="1">
+        <v>0.861302017300142</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" s="1">
         <v>2.5</v>
       </c>
       <c r="B77" s="1">
         <v>0.71337134848012795</v>
       </c>
-    </row>
-    <row r="78" spans="1:2">
+      <c r="C77" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D77" s="1">
+        <v>0.86795449576753603</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" s="1">
         <v>2.5333333333333301</v>
       </c>
       <c r="B78" s="1">
         <v>0.713925130514385</v>
       </c>
-    </row>
-    <row r="79" spans="1:2">
+      <c r="C78" s="1">
+        <v>2.5333333333333301</v>
+      </c>
+      <c r="D78" s="1">
+        <v>0.87464662598903198</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79" s="1">
         <v>2.5666666666666602</v>
       </c>
       <c r="B79" s="1">
         <v>0.71437362257172499</v>
       </c>
-    </row>
-    <row r="80" spans="1:2">
+      <c r="C79" s="1">
+        <v>2.5666666666666602</v>
+      </c>
+      <c r="D79" s="1">
+        <v>0.88125852475591104</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" s="1">
         <v>2.6</v>
       </c>
       <c r="B80" s="1">
         <v>0.71467205637373299</v>
       </c>
-    </row>
-    <row r="81" spans="1:2">
+      <c r="C80" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="D80" s="1">
+        <v>0.88774882637712804</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
       <c r="A81" s="1">
         <v>2.6333333333333302</v>
       </c>
       <c r="B81" s="1">
         <v>0.71503411936445904</v>
       </c>
-    </row>
-    <row r="82" spans="1:2">
+      <c r="C81" s="1">
+        <v>2.6333333333333302</v>
+      </c>
+      <c r="D81" s="1">
+        <v>0.89444399699666999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
       <c r="A82" s="1">
         <v>2.6666666666666599</v>
       </c>
       <c r="B82" s="1">
         <v>0.71516126596156504</v>
       </c>
-    </row>
-    <row r="83" spans="1:2">
+      <c r="C82" s="1">
+        <v>2.6666666666666599</v>
+      </c>
+      <c r="D82" s="1">
+        <v>0.90096092690643104</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83" s="1">
         <v>2.69999999999999</v>
       </c>
       <c r="B83" s="1">
         <v>0.71519868262275499</v>
       </c>
-    </row>
-    <row r="84" spans="1:2">
+      <c r="C83" s="1">
+        <v>2.69999999999999</v>
+      </c>
+      <c r="D83" s="1">
+        <v>0.90754690936952298</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
       <c r="A84" s="1">
         <v>2.7333333333333298</v>
       </c>
       <c r="B84" s="1">
         <v>0.71568750303071904</v>
       </c>
-    </row>
-    <row r="85" spans="1:2">
+      <c r="C84" s="1">
+        <v>2.7333333333333298</v>
+      </c>
+      <c r="D84" s="1">
+        <v>0.91432466122891998</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
       <c r="A85" s="1">
         <v>2.7666666666666599</v>
       </c>
       <c r="B85" s="1">
         <v>0.71570677381516401</v>
       </c>
-    </row>
-    <row r="86" spans="1:2">
+      <c r="C85" s="1">
+        <v>2.7666666666666599</v>
+      </c>
+      <c r="D85" s="1">
+        <v>0.92085285174496601</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
       <c r="A86" s="1">
         <v>2.7999999999999901</v>
       </c>
       <c r="B86" s="1">
         <v>0.71574097625038602</v>
       </c>
-    </row>
-    <row r="87" spans="1:2">
+      <c r="C86" s="1">
+        <v>2.7999999999999901</v>
+      </c>
+      <c r="D86" s="1">
+        <v>0.92719244810768597</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
       <c r="A87" s="1">
         <v>2.8333333333333299</v>
       </c>
       <c r="B87" s="1">
         <v>0.71573823570572903</v>
       </c>
-    </row>
-    <row r="88" spans="1:2">
+      <c r="C87" s="1">
+        <v>2.8333333333333299</v>
+      </c>
+      <c r="D87" s="1">
+        <v>0.93360412064278497</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
       <c r="A88" s="1">
         <v>2.86666666666666</v>
       </c>
       <c r="B88" s="1">
         <v>0.715793335249994</v>
       </c>
-    </row>
-    <row r="89" spans="1:2">
+      <c r="C88" s="1">
+        <v>2.86666666666666</v>
+      </c>
+      <c r="D88" s="1">
+        <v>0.94005807188708201</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
       <c r="A89" s="1">
         <v>2.8999999999999901</v>
       </c>
       <c r="B89" s="1">
         <v>0.71584047186500899</v>
       </c>
-    </row>
-    <row r="90" spans="1:2">
+      <c r="C89" s="1">
+        <v>2.8999999999999901</v>
+      </c>
+      <c r="D89" s="1">
+        <v>0.94656873190372404</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90" s="1">
         <v>2.93333333333333</v>
       </c>
       <c r="B90" s="1">
         <v>0.71578803776854605</v>
       </c>
-    </row>
-    <row r="91" spans="1:2">
+      <c r="C90" s="1">
+        <v>2.93333333333333</v>
+      </c>
+      <c r="D90" s="1">
+        <v>0.95284313108751795</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
       <c r="A91" s="1">
         <v>2.9666666666666601</v>
       </c>
       <c r="B91" s="1">
         <v>0.71595522359143104</v>
       </c>
-    </row>
-    <row r="92" spans="1:2">
+      <c r="C91" s="1">
+        <v>2.9666666666666601</v>
+      </c>
+      <c r="D91" s="1">
+        <v>0.95924001956170202</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
       <c r="A92" s="1">
         <v>3</v>
       </c>
       <c r="B92" s="1">
         <v>0.71612550167005895</v>
       </c>
-    </row>
-    <row r="93" spans="1:2">
+      <c r="C92" s="1">
+        <v>3</v>
+      </c>
+      <c r="D92" s="1">
+        <v>0.96564822429090102</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
       <c r="A93" s="1">
         <v>3.0333333333333301</v>
       </c>
       <c r="B93" s="1">
         <v>0.71610979906711603</v>
       </c>
-    </row>
-    <row r="94" spans="1:2">
+      <c r="C93" s="1">
+        <v>3.0333333333333301</v>
+      </c>
+      <c r="D93" s="1">
+        <v>0.97175890269107301</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
       <c r="A94" s="1">
         <v>3.0666666666666602</v>
       </c>
       <c r="B94" s="1">
         <v>0.71624266465437203</v>
       </c>
-    </row>
-    <row r="95" spans="1:2">
+      <c r="C94" s="1">
+        <v>3.0666666666666602</v>
+      </c>
+      <c r="D94" s="1">
+        <v>0.97793320094582703</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
       <c r="A95" s="1">
         <v>3.1</v>
       </c>
       <c r="B95" s="1">
         <v>0.71625743865386804</v>
       </c>
-    </row>
-    <row r="96" spans="1:2">
+      <c r="C95" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="D95" s="1">
+        <v>0.98373021882948897</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
       <c r="A96" s="1">
         <v>3.1333333333333302</v>
       </c>
       <c r="B96" s="1">
         <v>0.71627526728754798</v>
       </c>
-    </row>
-    <row r="97" spans="1:2">
+      <c r="C96" s="1">
+        <v>3.1333333333333302</v>
+      </c>
+      <c r="D96" s="1">
+        <v>0.99013033241258996</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97" s="1">
         <v>3.1666666666666599</v>
       </c>
       <c r="B97" s="1">
         <v>0.71625678154864303</v>
       </c>
-    </row>
-    <row r="98" spans="1:2">
+      <c r="C97" s="1">
+        <v>3.1666666666666599</v>
+      </c>
+      <c r="D97" s="1">
+        <v>0.99612213532582505</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
       <c r="A98" s="1">
         <v>3.19999999999999</v>
       </c>
       <c r="B98" s="1">
         <v>0.71628635367460802</v>
       </c>
-    </row>
-    <row r="99" spans="1:2">
+      <c r="C98" s="1">
+        <v>3.19999999999999</v>
+      </c>
+      <c r="D98" s="1">
+        <v>1.00249380335574</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
       <c r="A99" s="1">
         <v>3.2333333333333298</v>
       </c>
       <c r="B99" s="1">
         <v>0.71629530950607101</v>
       </c>
-    </row>
-    <row r="100" spans="1:2">
+      <c r="C99" s="1">
+        <v>3.2333333333333298</v>
+      </c>
+      <c r="D99" s="1">
+        <v>1.0082567680239001</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
       <c r="A100" s="1">
         <v>3.2666666666666599</v>
       </c>
       <c r="B100" s="1">
         <v>0.71629231827055395</v>
       </c>
-    </row>
-    <row r="101" spans="1:2">
+      <c r="C100" s="1">
+        <v>3.2666666666666599</v>
+      </c>
+      <c r="D100" s="1">
+        <v>1.01436887089346</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
       <c r="A101" s="1">
         <v>3.2999999999999901</v>
       </c>
       <c r="B101" s="1">
         <v>0.71632751601716205</v>
       </c>
-    </row>
-    <row r="102" spans="1:2">
+      <c r="C101" s="1">
+        <v>3.2999999999999901</v>
+      </c>
+      <c r="D101" s="1">
+        <v>1.0201506014619</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
       <c r="A102" s="1">
         <v>3.3333333333333299</v>
       </c>
       <c r="B102" s="1">
         <v>0.71633272131492298</v>
       </c>
-    </row>
-    <row r="103" spans="1:2">
+      <c r="C102" s="1">
+        <v>3.3333333333333299</v>
+      </c>
+      <c r="D102" s="1">
+        <v>1.02611303332548</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
       <c r="A103" s="1">
         <v>3.36666666666666</v>
       </c>
       <c r="B103" s="1">
         <v>0.71630745753457203</v>
       </c>
-    </row>
-    <row r="104" spans="1:2">
+      <c r="C103" s="1">
+        <v>3.36666666666666</v>
+      </c>
+      <c r="D103" s="1">
+        <v>1.03164497124215</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
       <c r="A104" s="1">
         <v>3.3999999999999901</v>
       </c>
       <c r="B104" s="1">
         <v>0.71629613305788997</v>
       </c>
-    </row>
-    <row r="105" spans="1:2">
+      <c r="C104" s="1">
+        <v>3.3999999999999901</v>
+      </c>
+      <c r="D104" s="1">
+        <v>1.0374091215969099</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
       <c r="A105" s="1">
         <v>3.43333333333333</v>
       </c>
       <c r="B105" s="1">
         <v>0.71639138449320305</v>
       </c>
-    </row>
-    <row r="106" spans="1:2">
+      <c r="C105" s="1">
+        <v>3.43333333333333</v>
+      </c>
+      <c r="D105" s="1">
+        <v>1.04324155944825</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
       <c r="A106" s="1">
         <v>3.4666666666666601</v>
       </c>
       <c r="B106" s="1">
         <v>0.71632140701368496</v>
       </c>
-    </row>
-    <row r="107" spans="1:2">
+      <c r="C106" s="1">
+        <v>3.4666666666666601</v>
+      </c>
+      <c r="D106" s="1">
+        <v>1.04900518085399</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
       <c r="A107" s="1">
         <v>3.5</v>
       </c>
       <c r="B107" s="1">
         <v>0.71630835448129204</v>
       </c>
-    </row>
-    <row r="108" spans="1:2">
+      <c r="C107" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="D107" s="1">
+        <v>1.0548634865209201</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
       <c r="A108" s="1">
         <v>3.5333333333333301</v>
       </c>
       <c r="B108" s="1">
         <v>0.71633772725561295</v>
       </c>
-    </row>
-    <row r="109" spans="1:2">
+      <c r="C108" s="1">
+        <v>3.5333333333333301</v>
+      </c>
+      <c r="D108" s="1">
+        <v>1.0601264154208601</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
       <c r="A109" s="1">
         <v>3.5666666666666602</v>
       </c>
       <c r="B109" s="1">
         <v>0.71635541203999997</v>
       </c>
-    </row>
-    <row r="110" spans="1:2">
+      <c r="C109" s="1">
+        <v>3.5666666666666602</v>
+      </c>
+      <c r="D109" s="1">
+        <v>1.0658053667505001</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
       <c r="A110" s="1">
         <v>3.6</v>
       </c>
       <c r="B110" s="1">
         <v>0.71644934695130602</v>
       </c>
-    </row>
-    <row r="111" spans="1:2">
+      <c r="C110" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="D110" s="1">
+        <v>1.07165580321009</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
       <c r="A111" s="1">
         <v>3.6333333333333302</v>
       </c>
       <c r="B111" s="1">
         <v>0.71678011756559601</v>
       </c>
-    </row>
-    <row r="112" spans="1:2">
+      <c r="C111" s="1">
+        <v>3.6333333333333302</v>
+      </c>
+      <c r="D111" s="1">
+        <v>1.07691290379954</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
       <c r="A112" s="1">
         <v>3.6666666666666599</v>
       </c>
       <c r="B112" s="1">
         <v>0.71672299905679504</v>
       </c>
-    </row>
-    <row r="113" spans="1:2">
+      <c r="C112" s="1">
+        <v>3.6666666666666599</v>
+      </c>
+      <c r="D112" s="1">
+        <v>1.0823487187823799</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
       <c r="A113" s="1">
         <v>3.69999999999999</v>
       </c>
       <c r="B113" s="1">
         <v>0.71679282140179401</v>
       </c>
-    </row>
-    <row r="114" spans="1:2">
+      <c r="C113" s="1">
+        <v>3.69999999999999</v>
+      </c>
+      <c r="D113" s="1">
+        <v>1.08783133275726</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
       <c r="A114" s="1">
         <v>3.7333333333333298</v>
       </c>
       <c r="B114" s="1">
         <v>0.71684608231264202</v>
       </c>
-    </row>
-    <row r="115" spans="1:2">
+      <c r="C114" s="1">
+        <v>3.7333333333333298</v>
+      </c>
+      <c r="D114" s="1">
+        <v>1.09314927914659</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
       <c r="A115" s="1">
         <v>3.7666666666666599</v>
       </c>
       <c r="B115" s="1">
         <v>0.716912937368411</v>
       </c>
-    </row>
-    <row r="116" spans="1:2">
+      <c r="C115" s="1">
+        <v>3.7666666666666599</v>
+      </c>
+      <c r="D115" s="1">
+        <v>1.0985691075839801</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
       <c r="A116" s="1">
         <v>3.7999999999999901</v>
       </c>
       <c r="B116" s="1">
         <v>0.71690244633668199</v>
       </c>
-    </row>
-    <row r="117" spans="1:2">
+      <c r="C116" s="1">
+        <v>3.7999999999999901</v>
+      </c>
+      <c r="D116" s="1">
+        <v>1.10411617919618</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
       <c r="A117" s="1">
         <v>3.8333333333333299</v>
       </c>
       <c r="B117" s="1">
         <v>0.71721614909035303</v>
       </c>
-    </row>
-    <row r="118" spans="1:2">
+      <c r="C117" s="1">
+        <v>3.8333333333333299</v>
+      </c>
+      <c r="D117" s="1">
+        <v>1.1092317500900599</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
       <c r="A118" s="1">
         <v>3.86666666666666</v>
       </c>
       <c r="B118" s="1">
         <v>0.71734341669344703</v>
       </c>
-    </row>
-    <row r="119" spans="1:2">
+      <c r="C118" s="1">
+        <v>3.86666666666666</v>
+      </c>
+      <c r="D118" s="1">
+        <v>1.11456086070239</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
       <c r="A119" s="1">
         <v>3.8999999999999901</v>
       </c>
       <c r="B119" s="1">
         <v>0.71739579859370095</v>
       </c>
-    </row>
-    <row r="120" spans="1:2">
+      <c r="C119" s="1">
+        <v>3.8999999999999901</v>
+      </c>
+      <c r="D119" s="1">
+        <v>1.1200803523764999</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
       <c r="A120" s="1">
         <v>3.93333333333333</v>
       </c>
       <c r="B120" s="1">
         <v>0.71791837421467397</v>
       </c>
-    </row>
-    <row r="121" spans="1:2">
+      <c r="C120" s="1">
+        <v>3.93333333333333</v>
+      </c>
+      <c r="D120" s="1">
+        <v>1.1252234569700701</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
       <c r="A121" s="1">
         <v>3.9666666666666601</v>
       </c>
       <c r="B121" s="1">
         <v>0.71752013067137999</v>
       </c>
-    </row>
-    <row r="122" spans="1:2">
+      <c r="C121" s="1">
+        <v>3.9666666666666601</v>
+      </c>
+      <c r="D121" s="1">
+        <v>1.1301583685324399</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
       <c r="A122" s="1">
         <v>4</v>
       </c>
       <c r="B122" s="1">
         <v>0.71747344118878797</v>
       </c>
-    </row>
-    <row r="123" spans="1:2">
+      <c r="C122" s="1">
+        <v>4</v>
+      </c>
+      <c r="D122" s="1">
+        <v>1.13515479623775</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
       <c r="A123" s="1">
         <v>4.0333333333333297</v>
       </c>
       <c r="B123" s="1">
         <v>0.71795145492633705</v>
       </c>
-    </row>
-    <row r="124" spans="1:2">
+      <c r="C123" s="1">
+        <v>4.0333333333333297</v>
+      </c>
+      <c r="D123" s="1">
+        <v>1.14048859276736</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
       <c r="A124" s="1">
         <v>4.0666666666666602</v>
       </c>
       <c r="B124" s="1">
         <v>0.71830503375542998</v>
       </c>
-    </row>
-    <row r="125" spans="1:2">
+      <c r="C124" s="1">
+        <v>4.0666666666666602</v>
+      </c>
+      <c r="D124" s="1">
+        <v>1.1455149038037999</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
       <c r="A125" s="1">
         <v>4.0999999999999996</v>
       </c>
       <c r="B125" s="1">
         <v>0.71895540615925202</v>
       </c>
-    </row>
-    <row r="126" spans="1:2">
+      <c r="C125" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D125" s="1">
+        <v>1.15092389956214</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
       <c r="A126" s="1">
         <v>4.1333333333333302</v>
       </c>
       <c r="B126" s="1">
         <v>0.71893660840256701</v>
       </c>
-    </row>
-    <row r="127" spans="1:2">
+      <c r="C126" s="1">
+        <v>4.1333333333333302</v>
+      </c>
+      <c r="D126" s="1">
+        <v>1.15534582348004</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
       <c r="A127" s="1">
         <v>4.1666666666666599</v>
       </c>
       <c r="B127" s="1">
         <v>0.71908050725102102</v>
       </c>
-    </row>
-    <row r="128" spans="1:2">
+      <c r="C127" s="1">
+        <v>4.1666666666666599</v>
+      </c>
+      <c r="D127" s="1">
+        <v>1.1602672290689899</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
       <c r="A128" s="1">
         <v>4.1999999999999904</v>
       </c>
       <c r="B128" s="1">
         <v>0.71911478793036898</v>
       </c>
-    </row>
-    <row r="129" spans="1:2">
+      <c r="C128" s="1">
+        <v>4.1999999999999904</v>
+      </c>
+      <c r="D128" s="1">
+        <v>1.16525622996331</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
       <c r="A129" s="1">
         <v>4.2333333333333298</v>
       </c>
       <c r="B129" s="1">
         <v>0.71939312087155904</v>
       </c>
-    </row>
-    <row r="130" spans="1:2">
+      <c r="C129" s="1">
+        <v>4.2333333333333298</v>
+      </c>
+      <c r="D129" s="1">
+        <v>1.1701046549477101</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
       <c r="A130" s="1">
         <v>4.2666666666666604</v>
       </c>
       <c r="B130" s="1">
         <v>0.71962773038958805</v>
       </c>
-    </row>
-    <row r="131" spans="1:2">
+      <c r="C130" s="1">
+        <v>4.2666666666666604</v>
+      </c>
+      <c r="D130" s="1">
+        <v>1.17502181542116</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
       <c r="A131" s="1">
         <v>4.2999999999999901</v>
       </c>
       <c r="B131" s="1">
         <v>0.71971967260964098</v>
       </c>
-    </row>
-    <row r="132" spans="1:2">
+      <c r="C131" s="1">
+        <v>4.2999999999999901</v>
+      </c>
+      <c r="D131" s="1">
+        <v>1.1794778715727099</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
       <c r="A132" s="1">
         <v>4.3333333333333304</v>
       </c>
       <c r="B132" s="1">
         <v>0.72010165792951997</v>
       </c>
-    </row>
-    <row r="133" spans="1:2">
+      <c r="C132" s="1">
+        <v>4.3333333333333304</v>
+      </c>
+      <c r="D132" s="1">
+        <v>1.18453008677126</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
       <c r="A133" s="1">
         <v>4.36666666666666</v>
       </c>
       <c r="B133" s="1">
         <v>0.72023980172897395</v>
       </c>
-    </row>
-    <row r="134" spans="1:2">
+      <c r="C133" s="1">
+        <v>4.36666666666666</v>
+      </c>
+      <c r="D133" s="1">
+        <v>1.18890364096837</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
       <c r="A134" s="1">
         <v>4.3999999999999897</v>
       </c>
       <c r="B134" s="1">
         <v>0.72166452154043903</v>
       </c>
-    </row>
-    <row r="135" spans="1:2">
+      <c r="C134" s="1">
+        <v>4.3999999999999897</v>
+      </c>
+      <c r="D134" s="1">
+        <v>1.1959638748888399</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
       <c r="A135" s="1">
         <v>4.43333333333333</v>
       </c>
       <c r="B135" s="1">
         <v>0.72056465961138905</v>
       </c>
-    </row>
-    <row r="136" spans="1:2">
+      <c r="C135" s="1">
+        <v>4.43333333333333</v>
+      </c>
+      <c r="D135" s="1">
+        <v>1.19825848273556</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
       <c r="A136" s="1">
         <v>4.4666666666666597</v>
       </c>
       <c r="B136" s="1">
         <v>0.72067648364540904</v>
+      </c>
+      <c r="C136" s="1">
+        <v>4.4666666666666597</v>
+      </c>
+      <c r="D136" s="1">
+        <v>1.2028964105690301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>